<commit_message>
- simplify progress things a little (now submit, note, mc_heading are treated as normal items) - no longer differentiate whether an item was one of answered, changed & valid, just require all three to count it.
</commit_message>
<xml_diff>
--- a/webroot/assets/example_surveys/dynamic_testsheet.xlsx
+++ b/webroot/assets/example_surveys/dynamic_testsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>optional</t>
   </si>
@@ -164,81 +164,106 @@
 3. Once you enter something here, progress should go up to 42%. It goes up less, because the item already contained a valid value.</t>
   </si>
   <si>
-    <t>1. This item should be seen.
-2. Progress should now be slightly different than before (at 21%), because these items were optional and weren't part of the progress calculation until now.
-3. Once you enter something (other than yay) here, progress should go up to 35%.</t>
-  </si>
-  <si>
-    <t>1. This item should be only be displayed if you enter "yay" into the first text box (do so now). 
+    <t>mc3</t>
+  </si>
+  <si>
+    <t>mc4</t>
+  </si>
+  <si>
+    <t>mc5</t>
+  </si>
+  <si>
+    <t>This item is just a simple yes/no item.</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>n5</t>
+  </si>
+  <si>
+    <t>Once you answer the items on this page, progress should go from 50% to 100%</t>
+  </si>
+  <si>
+    <t>mc6</t>
+  </si>
+  <si>
+    <t>If you finish hereafter, there's a bug.</t>
+  </si>
+  <si>
+    <t>This item was optional and is now shown. Progress should be at 90% and go up to 100% once you answer this item.</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>Finish (for real)</t>
+  </si>
+  <si>
+    <t>mc yes_no</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>mc0</t>
+  </si>
+  <si>
+    <t>This item is a special yes/no item, whose choices were generated using R.</t>
+  </si>
+  <si>
+    <t>`r 'YES (with R)'`</t>
+  </si>
+  <si>
+    <t>`r 'NO (with R)'`</t>
+  </si>
+  <si>
+    <t>This item should never be seen. `r stopifnot(!is.na(text1))`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `r stopifnot(!is.na(text1))`</t>
+  </si>
+  <si>
+    <t>1. This item should be only be displayed if you enter "yay" into the first text box.
 2. Once you've entered "yay", progress should go down (from 42 to 37.5%).
 3. Here you should be reading the value you added on page 0 __`r text0`__.
 4. Once you enter something here, progress should go up to 50%.</t>
   </si>
   <si>
-    <t>mc3</t>
-  </si>
-  <si>
-    <t>mc4</t>
-  </si>
-  <si>
-    <t>mc5</t>
-  </si>
-  <si>
-    <t>This item is just a simple yes/no item.</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>p5</t>
-  </si>
-  <si>
-    <t>n5</t>
-  </si>
-  <si>
-    <t>Once you answer the items on this page, progress should go from 50% to 100%</t>
-  </si>
-  <si>
-    <t>mc6</t>
-  </si>
-  <si>
-    <t>If you finish hereafter, there's a bug.</t>
-  </si>
-  <si>
-    <t>This item was optional and is now shown. Progress should be at 90% and go up to 100% once you answer this item.</t>
-  </si>
-  <si>
-    <t>p6</t>
-  </si>
-  <si>
-    <t>Finish (for real)</t>
-  </si>
-  <si>
-    <t>mc yes_no</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>mc0</t>
-  </si>
-  <si>
-    <t>This item is a special yes/no item, whose choices were generated using R.</t>
-  </si>
-  <si>
-    <t>`r 'YES (with R)'`</t>
-  </si>
-  <si>
-    <t>`r 'NO (with R)'`</t>
-  </si>
-  <si>
-    <t>This item should never be seen. `r stopifnot(!is.na(text1))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> `r stopifnot(!is.na(text1))`</t>
+    <t>1. This item should be seen.
+2. Progress should now be slightly different than before (at 21%), because these items were optional and weren't part of the progress calculation until now.
+3. Once you enter something (other than yay) here, progress should go up to 35%.
+4. Please now enter "yay" here, a new item should show up.</t>
+  </si>
+  <si>
+    <t>mmc1</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>text2 == "yay"</t>
+  </si>
+  <si>
+    <t>This item should never be seen. It has a showif referring to a hidden item on the same page, so it can never become true.</t>
+  </si>
+  <si>
+    <t>mmc2</t>
+  </si>
+  <si>
+    <t>mc_multiple</t>
+  </si>
+  <si>
+    <t>This item should never be seen. It has a showif referring to a hidden item on a previous page, so it can never become true.</t>
   </si>
 </sst>
 </file>
@@ -330,8 +355,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -513,15 +542,15 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -598,6 +627,8 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -674,6 +705,8 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1003,11 +1036,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1158,7 +1191,7 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1171,36 +1204,40 @@
     </row>
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="8" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="10" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="G9" s="8" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="18">
-      <c r="A10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>24</v>
+      <c r="A10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
         <v>15</v>
@@ -1209,266 +1246,306 @@
     </row>
     <row r="11" spans="1:8" ht="18">
       <c r="A11" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="10" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="126">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:8" ht="18">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="162">
+      <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1">
-      <c r="A13" s="13" t="s">
+    <row r="14" spans="1:8" ht="18" customHeight="1">
+      <c r="A14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="15" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-    </row>
     <row r="15" spans="1:8" ht="18" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" ht="162">
-      <c r="A16" s="8" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" customHeight="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" ht="144">
+      <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="2" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:8" ht="18">
+      <c r="A18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18">
-      <c r="A18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="10" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18">
+    <row r="19" spans="1:8" ht="18">
       <c r="A19" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45">
-      <c r="A20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30">
-      <c r="A21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18">
+      <c r="A20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18">
+      <c r="A21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="45">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30">
       <c r="A23" s="2" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45">
+        <v>48</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45">
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1508,13 +1585,13 @@
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
@@ -1522,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>